<commit_message>
display drivers to webpage
</commit_message>
<xml_diff>
--- a/Week2.xlsx
+++ b/Week2.xlsx
@@ -1325,7 +1325,12 @@
           <t>Monica</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Driver,
+Red Van</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
update number of days displayed
</commit_message>
<xml_diff>
--- a/Week2.xlsx
+++ b/Week2.xlsx
@@ -1325,7 +1325,12 @@
           <t>Monica</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Driver,
+Red Van</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
dont display employee_name under drivers
</commit_message>
<xml_diff>
--- a/Week2.xlsx
+++ b/Week2.xlsx
@@ -1325,12 +1325,7 @@
           <t>Monica</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Driver,
-Red Van</t>
-        </is>
-      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
remove other drivers from crew list
</commit_message>
<xml_diff>
--- a/Week2.xlsx
+++ b/Week2.xlsx
@@ -1325,7 +1325,12 @@
           <t>Monica</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Driver,
+Red Van</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>

</xml_diff>